<commit_message>
divide ipynb for steps
</commit_message>
<xml_diff>
--- a/AnalysisResult/RegressionResults.xlsx
+++ b/AnalysisResult/RegressionResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SBH\OneDrive - University College London\#CASA0007__QuantitativeMethods\ASSESSMENT\WrittenInvestigation\CASA0007A2QMBohaoSu\AnalysisResult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30916CCA-ABA8-47CF-9DC5-5CB6C6A1ED76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33A8D93-D01F-4A7B-93A0-6B1860224FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E0A62621-13BF-4EEC-906B-E6643A256AF8}"/>
   </bookViews>
@@ -1083,10 +1083,11 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'coef Compar'!$D$25:$I$25</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>'coef Compar'!$D$25:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2018</c:v>
                 </c:pt>
@@ -1102,18 +1103,15 @@
                 <c:pt idx="4">
                   <c:v>2022</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>SUM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coef Compar'!$D$26:$I$26</c:f>
+              <c:f>'coef Compar'!$D$26:$H$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.1147</c:v>
                 </c:pt>
@@ -1128,9 +1126,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.51949999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.1326</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1169,10 +1164,11 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'coef Compar'!$D$25:$I$25</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>'coef Compar'!$D$25:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2018</c:v>
                 </c:pt>
@@ -1188,18 +1184,15 @@
                 <c:pt idx="4">
                   <c:v>2022</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>SUM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coef Compar'!$D$27:$I$27</c:f>
+              <c:f>'coef Compar'!$D$27:$H$27</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>-0.2072</c:v>
                 </c:pt>
@@ -1214,9 +1207,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-0.1618</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-4.2200000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1255,10 +1245,11 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'coef Compar'!$D$25:$I$25</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>'coef Compar'!$D$25:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2018</c:v>
                 </c:pt>
@@ -1274,18 +1265,15 @@
                 <c:pt idx="4">
                   <c:v>2022</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>SUM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coef Compar'!$D$28:$I$28</c:f>
+              <c:f>'coef Compar'!$D$28:$H$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>-8.2000000000000007E-3</c:v>
                 </c:pt>
@@ -1300,9 +1288,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-0.32669999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.2437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1341,10 +1326,11 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'coef Compar'!$D$25:$I$25</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>'coef Compar'!$D$25:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2018</c:v>
                 </c:pt>
@@ -1360,18 +1346,15 @@
                 <c:pt idx="4">
                   <c:v>2022</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>SUM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coef Compar'!$D$29:$I$29</c:f>
+              <c:f>'coef Compar'!$D$29:$H$29</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>-0.18840000000000001</c:v>
                 </c:pt>
@@ -1386,9 +1369,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-0.26989999999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-3.7000000000000002E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1427,10 +1407,11 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'coef Compar'!$D$25:$I$25</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>'coef Compar'!$D$25:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2018</c:v>
                 </c:pt>
@@ -1446,18 +1427,15 @@
                 <c:pt idx="4">
                   <c:v>2022</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>SUM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coef Compar'!$D$30:$I$30</c:f>
+              <c:f>'coef Compar'!$D$30:$H$30</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>9.4000000000000004E-3</c:v>
                 </c:pt>
@@ -1472,9 +1450,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.3399999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.14319999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1513,10 +1488,11 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'coef Compar'!$D$25:$I$25</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>'coef Compar'!$D$25:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2018</c:v>
                 </c:pt>
@@ -1532,18 +1508,15 @@
                 <c:pt idx="4">
                   <c:v>2022</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>SUM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coef Compar'!$D$31:$I$31</c:f>
+              <c:f>'coef Compar'!$D$31:$H$31</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.3523</c:v>
                 </c:pt>
@@ -1558,9 +1531,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.31609999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.1086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,10 +1571,11 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>'coef Compar'!$D$25:$I$25</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>'coef Compar'!$D$25:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>2018</c:v>
                 </c:pt>
@@ -1620,18 +1591,15 @@
                 <c:pt idx="4">
                   <c:v>2022</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>SUM</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coef Compar'!$D$32:$I$32</c:f>
+              <c:f>'coef Compar'!$D$32:$H$32</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>-0.54469999999999996</c:v>
                 </c:pt>
@@ -1646,9 +1614,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-0.41930000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-7.9100000000000004E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3812,7 +3777,7 @@
   <dimension ref="C10:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4279,6 +4244,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010077CCD0EF0CC0C14D9BC56E0CF296901F" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b2739cee47380b412252b0a7f7b46cdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="36cefabe-3f9c-4b7e-957f-c04dcb44e569" xmlns:ns4="e3ae1f4c-d6c7-4409-b438-ba19ee4924f8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7593055570ed88eb1fa099247007281e" ns3:_="" ns4:_="">
     <xsd:import namespace="36cefabe-3f9c-4b7e-957f-c04dcb44e569"/>
@@ -4505,15 +4479,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4523,6 +4488,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CA184A6-7451-4B59-845A-21AFB1F0B5D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE444B81-6678-4DE5-815C-7790D36A6DF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4537,14 +4510,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CA184A6-7451-4B59-845A-21AFB1F0B5D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>